<commit_message>
fixed crash when profs with no areas/projects are clicked on
</commit_message>
<xml_diff>
--- a/Cos Department Data.xlsx
+++ b/Cos Department Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ptaylor/Documents/advisor-search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCE5851D-9FC2-9E45-BEAB-F4E5EFC393F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6328C7-5418-D24A-B841-E50936E8561E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1110,7 +1110,7 @@
   <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B52" sqref="B52"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>